<commit_message>
Cosmetic changes, foundation of the app developed
</commit_message>
<xml_diff>
--- a/assets/data_sources.xlsx
+++ b/assets/data_sources.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shiny.cucumber\projects\dashboarddb\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shiny.cucumber\projects\ukraine_data\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18C9226-A709-4D39-BDFB-CBD047D433AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEABE29E-ABC3-45B7-BE1A-57ADC97ECD48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5484" yWindow="2244" windowWidth="16440" windowHeight="9372" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2964" yWindow="2964" windowWidth="16440" windowHeight="9372" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sources" sheetId="1" r:id="rId1"/>
@@ -325,9 +325,6 @@
     <t>Income from capital transactions</t>
   </si>
   <si>
-    <t>Receipts from the European Union, the governments of foreign countries and international organizations</t>
-  </si>
-  <si>
     <t>Targeted  funds</t>
   </si>
   <si>
@@ -430,12 +427,6 @@
     <t>External financing</t>
   </si>
   <si>
-    <t>Loans granted by international financial institutions</t>
-  </si>
-  <si>
-    <t>Loans granted by governments of foreign countries</t>
-  </si>
-  <si>
     <t>Loans granted by foreign commercial banks and other foreign financial institutions</t>
   </si>
   <si>
@@ -475,24 +466,9 @@
     <t>Domestic Loans returned</t>
   </si>
   <si>
-    <t>Consumer price indices (to corresponding month of the previous year, %)</t>
-  </si>
-  <si>
-    <t>Food  and non-alcoholic beverages</t>
-  </si>
-  <si>
-    <t>Alcoholic beverages, tobacco</t>
-  </si>
-  <si>
     <t>Clothing and footwear</t>
   </si>
   <si>
-    <t>Housing, water,  electricity,  gas and other fuels</t>
-  </si>
-  <si>
-    <t>Furnishings, household equipment and routine maintenance of the house</t>
-  </si>
-  <si>
     <t>Health</t>
   </si>
   <si>
@@ -508,9 +484,6 @@
     <t>Restaurants and hotels</t>
   </si>
   <si>
-    <t>Miscellaneous goods and services</t>
-  </si>
-  <si>
     <t>Official reserve assets</t>
   </si>
   <si>
@@ -704,6 +677,33 @@
   </si>
   <si>
     <t>Nationals: average</t>
+  </si>
+  <si>
+    <t>Food and non-alcoholic drinks</t>
+  </si>
+  <si>
+    <t>Alcoholic drinks, tobacco</t>
+  </si>
+  <si>
+    <t>Housing, water, electricity, fuels</t>
+  </si>
+  <si>
+    <t>Other goods and services</t>
+  </si>
+  <si>
+    <t>Inflation, yoy</t>
+  </si>
+  <si>
+    <t>House appliances, furniture, maintenance</t>
+  </si>
+  <si>
+    <t>Receipts from the EU, foreign governments and international organizations</t>
+  </si>
+  <si>
+    <t>International organisations</t>
+  </si>
+  <si>
+    <t>Foreign governments</t>
   </si>
 </sst>
 </file>
@@ -1145,7 +1145,7 @@
         <v>21</v>
       </c>
       <c r="H1" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1434,7 +1434,7 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>46</v>
@@ -1457,7 +1457,7 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>46</v>
@@ -1480,7 +1480,7 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>46</v>
@@ -1702,8 +1702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC56B33F-EF9E-43A0-B1C8-80B283EAD1FB}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="A2:XFD2"/>
+    <sheetView topLeftCell="A15" zoomScale="85" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1713,21 +1713,21 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B1" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="C1" t="s">
         <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2130,7 +2130,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>93</v>
+        <v>217</v>
       </c>
       <c r="B31">
         <v>42000000</v>
@@ -2144,7 +2144,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B32">
         <v>50000000</v>
@@ -2173,21 +2173,21 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B1" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="C1" t="s">
         <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -2201,7 +2201,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B3">
         <v>200</v>
@@ -2215,7 +2215,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B4">
         <v>300</v>
@@ -2229,7 +2229,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B5">
         <v>400</v>
@@ -2243,7 +2243,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B6">
         <v>500</v>
@@ -2257,7 +2257,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B7">
         <v>600</v>
@@ -2271,7 +2271,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B8">
         <v>700</v>
@@ -2285,7 +2285,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B9">
         <v>800</v>
@@ -2299,7 +2299,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B10">
         <v>900</v>
@@ -2313,7 +2313,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B11">
         <v>1000</v>
@@ -2327,7 +2327,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -2338,7 +2338,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B13">
         <v>180</v>
@@ -2352,7 +2352,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -2363,7 +2363,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B15">
         <v>2000</v>
@@ -2377,7 +2377,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B16">
         <v>2100</v>
@@ -2391,7 +2391,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B17">
         <v>2200</v>
@@ -2405,7 +2405,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B18">
         <v>2400</v>
@@ -2419,7 +2419,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B19">
         <v>2600</v>
@@ -2433,7 +2433,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B20">
         <v>2700</v>
@@ -2447,7 +2447,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B21">
         <v>2800</v>
@@ -2461,7 +2461,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B22">
         <v>3000</v>
@@ -2475,7 +2475,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B23">
         <v>3100</v>
@@ -2489,7 +2489,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B24">
         <v>3200</v>
@@ -2503,7 +2503,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -2521,29 +2521,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8FBB677-25A5-40D2-9887-B5212FAAC09C}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D3:D32"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="37.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B1" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="C1" t="s">
         <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2554,7 +2555,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B3">
         <v>200000</v>
@@ -2568,7 +2569,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B4">
         <v>202000</v>
@@ -2582,7 +2583,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B5">
         <v>203000</v>
@@ -2596,7 +2597,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B6">
         <v>204000</v>
@@ -2610,7 +2611,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B7">
         <v>205000</v>
@@ -2624,7 +2625,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B8">
         <v>206000</v>
@@ -2638,7 +2639,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B9">
         <v>207000</v>
@@ -2652,7 +2653,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B10">
         <v>208000</v>
@@ -2666,7 +2667,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B11">
         <v>300000</v>
@@ -2680,7 +2681,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>128</v>
+        <v>218</v>
       </c>
       <c r="B12">
         <v>301000</v>
@@ -2694,7 +2695,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>129</v>
+        <v>219</v>
       </c>
       <c r="B13">
         <v>302000</v>
@@ -2708,7 +2709,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B14">
         <v>303000</v>
@@ -2722,7 +2723,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B15">
         <v>304000</v>
@@ -2736,7 +2737,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B16">
         <v>305000</v>
@@ -2750,7 +2751,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B17">
         <v>307000</v>
@@ -2764,7 +2765,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -2775,7 +2776,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B19">
         <v>400000</v>
@@ -2789,7 +2790,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B20">
         <v>401000</v>
@@ -2803,7 +2804,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B21">
         <v>402000</v>
@@ -2817,7 +2818,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B22">
         <v>403000</v>
@@ -2831,7 +2832,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B23">
         <v>500000</v>
@@ -2845,7 +2846,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B24">
         <v>600000</v>
@@ -2859,7 +2860,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B25">
         <v>601000</v>
@@ -2873,7 +2874,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B26">
         <v>602000</v>
@@ -2887,7 +2888,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B27">
         <v>603000</v>
@@ -2901,7 +2902,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -2912,7 +2913,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -2923,7 +2924,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B30">
         <v>4000</v>
@@ -2937,7 +2938,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B31">
         <v>4110</v>
@@ -2951,7 +2952,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B32">
         <v>4120</v>
@@ -2973,22 +2974,25 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B14"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="35.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B1" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>215</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -2996,7 +3000,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>211</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
@@ -3004,7 +3008,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>145</v>
+        <v>212</v>
       </c>
       <c r="B4" t="b">
         <v>0</v>
@@ -3012,7 +3016,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
@@ -3020,7 +3024,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>147</v>
+        <v>213</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
@@ -3028,7 +3032,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>148</v>
+        <v>216</v>
       </c>
       <c r="B7" t="b">
         <v>0</v>
@@ -3036,7 +3040,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B8" t="b">
         <v>0</v>
@@ -3044,7 +3048,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B9" t="b">
         <v>0</v>
@@ -3052,7 +3056,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B10" t="b">
         <v>0</v>
@@ -3060,7 +3064,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B11" t="b">
         <v>0</v>
@@ -3068,7 +3072,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B12" t="b">
         <v>0</v>
@@ -3076,7 +3080,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B13" t="b">
         <v>0</v>
@@ -3084,7 +3088,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>154</v>
+        <v>214</v>
       </c>
       <c r="B14" t="b">
         <v>0</v>
@@ -3107,15 +3111,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B1" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -3123,7 +3127,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
@@ -3131,7 +3135,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B4" t="b">
         <v>0</v>
@@ -3139,7 +3143,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
@@ -3147,7 +3151,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
@@ -3155,7 +3159,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B7" t="b">
         <v>0</v>
@@ -3181,7 +3185,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B1" t="s">
         <v>32</v>
@@ -3189,7 +3193,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3197,7 +3201,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3205,7 +3209,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3213,7 +3217,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -3221,7 +3225,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -3229,7 +3233,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3237,7 +3241,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3245,7 +3249,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3253,7 +3257,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3261,7 +3265,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3269,7 +3273,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3277,7 +3281,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3285,7 +3289,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3293,7 +3297,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -3301,7 +3305,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -3309,7 +3313,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -3317,7 +3321,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -3325,7 +3329,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -3333,7 +3337,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -3341,7 +3345,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -3349,7 +3353,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -3357,7 +3361,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -3365,7 +3369,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -3373,7 +3377,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -3381,7 +3385,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -3389,7 +3393,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -3397,7 +3401,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -3405,7 +3409,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -3413,7 +3417,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -3421,7 +3425,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -3429,7 +3433,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -3437,7 +3441,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -3445,7 +3449,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -3453,7 +3457,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -3461,7 +3465,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -3496,7 +3500,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B1" t="s">
         <v>32</v>
@@ -3504,7 +3508,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3512,7 +3516,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3520,7 +3524,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3528,7 +3532,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -3536,7 +3540,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -3544,7 +3548,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -3552,7 +3556,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -3560,7 +3564,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3568,7 +3572,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -3576,7 +3580,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -3584,7 +3588,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -3599,7 +3603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{591E5F52-587D-419F-A27E-3AF6EE242237}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -3611,7 +3615,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B1" t="s">
         <v>32</v>
@@ -3619,7 +3623,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3627,7 +3631,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -3635,7 +3639,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -3643,7 +3647,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3651,7 +3655,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -3659,7 +3663,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -3667,7 +3671,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3675,7 +3679,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3683,7 +3687,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -3691,7 +3695,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="B11">
         <v>0</v>

</xml_diff>

<commit_message>
All metrics added, added labels to barchart graphs,, expanders added
</commit_message>
<xml_diff>
--- a/assets/data_sources.xlsx
+++ b/assets/data_sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shiny.cucumber\projects\ukraine_data\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6A6538-3B5B-4B8B-B5F9-96B601357417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D8B3F4-3683-4AC9-A420-D91DDB5A23E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2664" windowWidth="21924" windowHeight="10296" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sources" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="366">
   <si>
     <t>source</t>
   </si>
@@ -1136,6 +1136,21 @@
   </si>
   <si>
     <t>Delivered military help</t>
+  </si>
+  <si>
+    <t>tf_gdp_ua.csv</t>
+  </si>
+  <si>
+    <t>GDP Ukraine, current USD</t>
+  </si>
+  <si>
+    <t>World Bank (Dbnomics)</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>https://api.db.nomics.world/v22/series/WB/WDI/A-NY.GDP.MKTP.CD-UKR.csv</t>
   </si>
 </sst>
 </file>
@@ -2248,10 +2263,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55CAA2C0-DB42-4D84-A6A6-1D10E6E62173}">
-  <dimension ref="A1:N56"/>
+  <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3996,9 +4011,53 @@
         <v>0</v>
       </c>
     </row>
+    <row r="57" spans="1:14">
+      <c r="A57" t="s">
+        <v>361</v>
+      </c>
+      <c r="B57" t="s">
+        <v>227</v>
+      </c>
+      <c r="C57" t="s">
+        <v>225</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57" t="s">
+        <v>362</v>
+      </c>
+      <c r="G57" t="s">
+        <v>300</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="I57" t="s">
+        <v>326</v>
+      </c>
+      <c r="J57" t="s">
+        <v>364</v>
+      </c>
+      <c r="K57">
+        <v>2021</v>
+      </c>
+      <c r="L57" t="s">
+        <v>344</v>
+      </c>
+      <c r="M57" t="s">
+        <v>363</v>
+      </c>
+      <c r="N57" t="s">
+        <v>365</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>